<commit_message>
code test_scenario change and fix gui
fix gui input_actual and change code test_scenario to respon in future
</commit_message>
<xml_diff>
--- a/testsheet_lab.xlsx
+++ b/testsheet_lab.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\นัท\Python\pytest_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5AC0D78-155B-40A0-8989-900D9023294F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0FCC0A1-73D7-45C4-AE49-9D1EE77B6B96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -714,8 +714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -727,8 +727,8 @@
     <col min="8" max="8" width="10.25" style="2" customWidth="1"/>
     <col min="9" max="9" width="41.75" style="2" customWidth="1"/>
     <col min="10" max="10" width="20.75" style="2" customWidth="1"/>
-    <col min="11" max="62" width="8.875" style="2" customWidth="1"/>
-    <col min="63" max="16384" width="8.875" style="2"/>
+    <col min="11" max="72" width="8.875" style="2" customWidth="1"/>
+    <col min="73" max="16384" width="8.875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -1015,7 +1015,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="H22" sqref="H21:H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1025,8 +1025,8 @@
     <col min="8" max="8" width="10.25" style="2" customWidth="1"/>
     <col min="9" max="9" width="41.75" style="2" customWidth="1"/>
     <col min="10" max="10" width="20.75" style="2" customWidth="1"/>
-    <col min="11" max="62" width="8.875" style="2" customWidth="1"/>
-    <col min="63" max="16384" width="8.875" style="2"/>
+    <col min="11" max="72" width="8.875" style="2" customWidth="1"/>
+    <col min="73" max="16384" width="8.875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>